<commit_message>
Happy New Year Update
</commit_message>
<xml_diff>
--- a/doc/Fermi Main.xlsx
+++ b/doc/Fermi Main.xlsx
@@ -9,14 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="10632" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19365" windowHeight="10635" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Go" sheetId="1" r:id="rId1"/>
     <sheet name="Dati" sheetId="2" r:id="rId2"/>
-    <sheet name="Distances" sheetId="3" r:id="rId3"/>
-    <sheet name="More Distances" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId5"/>
+    <sheet name="More Distances" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Dpi.f1">Dati!$B$18</definedName>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="108">
   <si>
     <t>Fel1Factor</t>
   </si>
@@ -216,24 +215,6 @@
     <t>PM1b</t>
   </si>
   <si>
-    <t>TMR</t>
-  </si>
-  <si>
-    <t>Trinity</t>
-  </si>
-  <si>
-    <t>Coh Slit</t>
-  </si>
-  <si>
-    <t>Coh CCD</t>
-  </si>
-  <si>
-    <t>Deltas</t>
-  </si>
-  <si>
-    <t>Coh Slits</t>
-  </si>
-  <si>
     <t>PRESTO</t>
   </si>
   <si>
@@ -246,9 +227,6 @@
     <t>VDM</t>
   </si>
   <si>
-    <t>DIP</t>
-  </si>
-  <si>
     <t>KBV</t>
   </si>
   <si>
@@ -256,9 +234,6 @@
   </si>
   <si>
     <t>h</t>
-  </si>
-  <si>
-    <t>2?</t>
   </si>
   <si>
     <t>PreviousElement</t>
@@ -909,55 +884,55 @@
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:2" s="14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
     </row>
-    <row r="9" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -965,7 +940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -973,7 +948,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -982,7 +957,7 @@
         <v>2.5000000000000002E-8</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -991,7 +966,7 @@
         <v>3.7499999999999997E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1000,7 +975,7 @@
         <v>2.1220659078919382E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
@@ -1009,7 +984,7 @@
         <v>1.5005271935951769E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
@@ -1018,7 +993,7 @@
         <v>1.5005271935951769E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>30</v>
       </c>
@@ -1028,12 +1003,12 @@
       </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
@@ -1041,7 +1016,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1050,7 +1025,7 @@
         <v>2.6249999999999997E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>6</v>
       </c>
@@ -1059,12 +1034,12 @@
         <v>6.1687499999999998E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>34</v>
       </c>
@@ -1072,7 +1047,7 @@
         <v>98.5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -1087,7 +1062,7 @@
         <v>58.333333333333336</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
@@ -1102,7 +1077,7 @@
         <v>2.5723323318774461E-6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>21</v>
       </c>
@@ -1110,7 +1085,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -1119,7 +1094,7 @@
         <v>3.6937499999999996E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -1128,7 +1103,7 @@
         <v>5.2767857142857148E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>39</v>
       </c>
@@ -1137,7 +1112,7 @@
         <v>1.2400446428571431E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>49</v>
       </c>
@@ -1146,7 +1121,7 @@
         <v>68.891369047619051</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D42">
         <f>11/2.5</f>
         <v>4.4000000000000004</v>
@@ -1163,23 +1138,23 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" style="8" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
@@ -1187,7 +1162,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
@@ -1195,7 +1170,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>12</v>
       </c>
@@ -1203,13 +1178,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>40</v>
       </c>
@@ -1217,7 +1192,7 @@
         <v>84.846599999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
@@ -1225,7 +1200,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>41</v>
       </c>
@@ -1233,13 +1208,13 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>17</v>
       </c>
@@ -1247,7 +1222,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>19</v>
       </c>
@@ -1256,7 +1231,7 @@
         <v>4.3611111111111114E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>18</v>
       </c>
@@ -1265,7 +1240,7 @@
         <v>1.7438915287774956E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>20</v>
       </c>
@@ -1273,17 +1248,17 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B17" s="22"/>
       <c r="D17" s="12" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E17" s="10"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>9</v>
       </c>
@@ -1298,7 +1273,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>10</v>
       </c>
@@ -1312,22 +1287,22 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B20">
         <v>98.55</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E20">
         <f>Dpi.f2H-B4</f>
         <v>91.55</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>8</v>
       </c>
@@ -1341,7 +1316,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>41</v>
       </c>
@@ -1349,13 +1324,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>35</v>
       </c>
@@ -1363,7 +1338,7 @@
         <v>74.442700000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>36</v>
       </c>
@@ -1371,7 +1346,7 @@
         <v>6.5919999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>37</v>
       </c>
@@ -1379,7 +1354,7 @@
         <v>76.932900000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>38</v>
       </c>
@@ -1387,12 +1362,12 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>32</v>
       </c>
@@ -1408,301 +1383,59 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="B1:R39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3">
-        <v>48.0901</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4">
-        <v>41.442700000000002</v>
-      </c>
-      <c r="E4">
-        <f>D4-D2</f>
-        <v>41.442700000000002</v>
-      </c>
-      <c r="F4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5">
-        <v>54.328899999999997</v>
-      </c>
-      <c r="D5">
-        <v>46.6815</v>
-      </c>
-      <c r="J5">
-        <f>D5-D4</f>
-        <v>5.2387999999999977</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6">
-        <v>57.494</v>
-      </c>
-      <c r="D6">
-        <v>49.846600000000002</v>
-      </c>
-      <c r="J6">
-        <f t="shared" ref="J6:J15" si="0">D6-D5</f>
-        <v>3.1651000000000025</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7">
-        <v>77.494</v>
-      </c>
-      <c r="D7">
-        <v>69.846599999999995</v>
-      </c>
-      <c r="E7">
-        <f>D7-D4</f>
-        <v>28.403899999999993</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="0"/>
-        <v>19.999999999999993</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>-69.846599999999995</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10">
-        <v>58.748699999999999</v>
-      </c>
-      <c r="D10">
-        <v>66.396000000000001</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>66.396000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11">
-        <v>74.668000000000006</v>
-      </c>
-      <c r="D11">
-        <v>67.020600000000002</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
-        <v>0.62460000000000093</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12">
-        <f>C11+(1380+100+1000.7+900+5143.8)/1000</f>
-        <v>83.19250000000001</v>
-      </c>
-      <c r="H12" t="s">
-        <v>61</v>
-      </c>
-      <c r="I12">
-        <f>C12-C10</f>
-        <v>24.44380000000001</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
-        <v>-67.020600000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14">
-        <v>94.494</v>
-      </c>
-      <c r="D14">
-        <v>86.846599999999995</v>
-      </c>
-      <c r="E14">
-        <f>D14-D7</f>
-        <v>17</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="0"/>
-        <v>86.846599999999995</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15">
-        <v>98.5</v>
-      </c>
-      <c r="D15">
-        <v>98</v>
-      </c>
-      <c r="E15">
-        <f>D15-D7</f>
-        <v>28.153400000000005</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="0"/>
-        <v>11.153400000000005</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R39"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="6" max="6" width="21.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
     <col min="9" max="9" width="17" style="24" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" style="24" customWidth="1"/>
     <col min="11" max="11" width="16" style="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="K1" s="27" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>53</v>
       </c>
@@ -1710,16 +1443,16 @@
         <v>2.5</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F3">
         <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I3" s="24">
         <v>48.0901</v>
@@ -1729,7 +1462,7 @@
       </c>
       <c r="R3" s="18"/>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>55</v>
       </c>
@@ -1737,16 +1470,16 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F4">
         <v>50</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I4" s="24">
         <v>54.328899999999997</v>
@@ -1758,7 +1491,7 @@
       <c r="O4" s="19"/>
       <c r="Q4" s="20"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>54</v>
       </c>
@@ -1766,30 +1499,30 @@
         <v>2.5</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F5">
         <v>50</v>
       </c>
       <c r="G5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="K5" s="27">
         <v>41.442700000000002</v>
       </c>
       <c r="M5" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="N5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F6">
         <v>50</v>
@@ -1797,47 +1530,47 @@
       <c r="O6" s="20"/>
       <c r="Q6" s="20"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F7">
         <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="R8" s="18"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C9">
         <v>2.5</v>
       </c>
       <c r="D9" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F9">
         <v>50</v>
       </c>
       <c r="G9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I9" s="24">
         <v>57.494</v>
@@ -1849,25 +1582,29 @@
       <c r="K9" s="27">
         <v>49.846600000000002</v>
       </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="O9">
+        <f>K9-K37</f>
+        <v>-48.703399999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C10">
         <v>2.5</v>
       </c>
       <c r="D10" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F10">
         <v>50</v>
       </c>
       <c r="G10" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I10" s="24">
         <v>57.494</v>
@@ -1876,24 +1613,24 @@
         <v>49.846600000000002</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C11">
         <v>2.5</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F11">
         <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I11" s="24">
         <v>57.494</v>
@@ -1902,27 +1639,27 @@
         <v>49.846600000000002</v>
       </c>
       <c r="N11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E13" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F13">
         <v>50</v>
       </c>
       <c r="G13" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I13" s="24">
         <v>77.494</v>
@@ -1931,32 +1668,32 @@
         <v>69.846599999999995</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F14">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E15" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F15">
         <v>50</v>
       </c>
       <c r="G15" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I15" s="24">
         <v>77.494</v>
@@ -1965,32 +1702,32 @@
         <v>69.846599999999995</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F16">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E18" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F18">
         <v>40</v>
       </c>
       <c r="G18" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="I18" s="24">
         <v>94.494</v>
@@ -1999,35 +1736,35 @@
         <v>86.846599999999995</v>
       </c>
       <c r="N18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F19">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E20" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F20">
         <v>30</v>
       </c>
       <c r="G20" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="I20" s="24">
         <v>98.5</v>
@@ -2036,269 +1773,272 @@
         <v>98</v>
       </c>
       <c r="N20" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F21">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E22" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F22">
         <v>30</v>
       </c>
       <c r="G22" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="K22" s="27">
-        <v>98.55</v>
+        <v>91.55</v>
       </c>
       <c r="L22">
         <f>K22-K9</f>
-        <v>48.703399999999995</v>
+        <v>41.703399999999995</v>
       </c>
       <c r="N22" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F23">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C25">
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E25" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F25">
         <v>40</v>
       </c>
       <c r="G25" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F26">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E27" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F27">
         <v>30</v>
       </c>
       <c r="G27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F28">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E29" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F29">
         <v>30</v>
       </c>
       <c r="G29" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F30">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C32">
         <v>2.5</v>
       </c>
       <c r="D32" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E32" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F32">
         <v>40</v>
       </c>
       <c r="G32" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E34" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F34">
         <v>40</v>
       </c>
       <c r="G34" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E35" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F35">
         <v>40</v>
       </c>
       <c r="G35" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="M35" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C37">
         <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E37" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F37">
         <v>30</v>
       </c>
       <c r="G37" t="s">
-        <v>69</v>
+        <v>62</v>
+      </c>
+      <c r="K37" s="25">
+        <v>98.55</v>
       </c>
       <c r="M37" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C38">
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E38" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F38">
         <v>30</v>
       </c>
       <c r="G38" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="M38" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C39">
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E39" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F39">
         <v>30</v>
       </c>
       <c r="G39" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="M39" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2307,7 +2047,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -2315,12 +2055,12 @@
       <selection sqref="A1:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>51</v>
       </c>
@@ -2328,10 +2068,10 @@
         <v>52</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
         <v>11</v>
       </c>
@@ -2339,7 +2079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>53</v>
       </c>
@@ -2347,7 +2087,7 @@
         <v>48.0901</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>54</v>
       </c>
@@ -2359,9 +2099,9 @@
         <v>41.442700000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C5">
         <v>57.494</v>
@@ -2370,9 +2110,9 @@
         <v>49.846600000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C6">
         <v>77.494</v>
@@ -2385,12 +2125,12 @@
         <v>28.403899999999993</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C7">
         <v>94.494</v>
@@ -2403,12 +2143,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C8">
         <v>98.5</v>
@@ -2421,9 +2161,9 @@
         <v>4.1534000000000049</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D9" s="20">
         <v>91.55</v>

</xml_diff>

<commit_message>
FileIO => added H%
</commit_message>
<xml_diff>
--- a/doc/Fermi Main.xlsx
+++ b/doc/Fermi Main.xlsx
@@ -9,33 +9,33 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="10632" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19365" windowHeight="10500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Go" sheetId="1" r:id="rId1"/>
-    <sheet name="Dati" sheetId="2" r:id="rId2"/>
+    <sheet name="Focussing Distances" sheetId="2" r:id="rId2"/>
     <sheet name="More Distances" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Dpi.f1">Dati!$B$18</definedName>
-    <definedName name="Dpi.f1V">Dati!$B$18</definedName>
-    <definedName name="Dpi.f2H">Dati!$B$20</definedName>
-    <definedName name="Dpi.f2V">Dati!$B$21</definedName>
-    <definedName name="Fel1Factor">Dati!$B$2</definedName>
-    <definedName name="Fel2Factor">Dati!$B$3</definedName>
+    <definedName name="Dpi.f1">'Focussing Distances'!$B$18</definedName>
+    <definedName name="Dpi.f1V">'Focussing Distances'!$B$18</definedName>
+    <definedName name="Dpi.f2H">'Focussing Distances'!$B$20</definedName>
+    <definedName name="Dpi.f2V">'Focussing Distances'!$B$21</definedName>
+    <definedName name="Fel1Factor">'Focussing Distances'!$B$2</definedName>
+    <definedName name="Fel2Factor">'Focussing Distances'!$B$3</definedName>
     <definedName name="FelSource">Go!$B$10</definedName>
-    <definedName name="Kb.AngleIn">Dati!$B$13</definedName>
-    <definedName name="Kb.CrossSection">Dati!$B$14</definedName>
-    <definedName name="Kb.Size">Dati!$B$14</definedName>
+    <definedName name="Kb.AngleIn">'Focussing Distances'!$B$13</definedName>
+    <definedName name="Kb.CrossSection">'Focussing Distances'!$B$14</definedName>
+    <definedName name="Kb.Size">'Focussing Distances'!$B$14</definedName>
     <definedName name="Lambda">Go!$B$12</definedName>
     <definedName name="Lambda_nm">Go!$B$11</definedName>
     <definedName name="ThetaI">Go!$B$13</definedName>
-    <definedName name="Tmx.f1">Dati!$B$7</definedName>
-    <definedName name="Tmx.f2">Dati!$B$8</definedName>
+    <definedName name="Tmx.f1">'Focussing Distances'!$B$7</definedName>
+    <definedName name="Tmx.f2">'Focussing Distances'!$B$8</definedName>
     <definedName name="z">Go!$B$21</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="114">
   <si>
     <t>Fel1Factor</t>
   </si>
@@ -375,14 +375,27 @@
   </si>
   <si>
     <t>F2 Source</t>
+  </si>
+  <si>
+    <t>Coherence: slit</t>
+  </si>
+  <si>
+    <t>Coherence: CCD</t>
+  </si>
+  <si>
+    <t>Yag: Pos-2</t>
+  </si>
+  <si>
+    <t>EIS SWITCHING</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -565,7 +578,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -609,6 +622,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Bad" xfId="6" builtinId="27"/>
@@ -901,55 +915,55 @@
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:2" s="14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
     </row>
-    <row r="9" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -957,7 +971,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -965,7 +979,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -974,7 +988,7 @@
         <v>2.5000000000000002E-8</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -983,7 +997,7 @@
         <v>3.7499999999999997E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -992,7 +1006,7 @@
         <v>2.1220659078919382E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
@@ -1001,7 +1015,7 @@
         <v>1.5005271935951769E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
@@ -1010,7 +1024,7 @@
         <v>1.5005271935951769E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>30</v>
       </c>
@@ -1020,12 +1034,12 @@
       </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
@@ -1033,7 +1047,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1042,7 +1056,7 @@
         <v>2.6249999999999997E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>6</v>
       </c>
@@ -1051,12 +1065,12 @@
         <v>6.1687499999999998E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>34</v>
       </c>
@@ -1064,7 +1078,7 @@
         <v>98.5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -1079,7 +1093,7 @@
         <v>58.333333333333336</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
@@ -1094,7 +1108,7 @@
         <v>2.5723323318774461E-6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>21</v>
       </c>
@@ -1102,7 +1116,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -1111,7 +1125,7 @@
         <v>3.6937499999999996E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -1120,7 +1134,7 @@
         <v>5.2767857142857148E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>39</v>
       </c>
@@ -1129,7 +1143,7 @@
         <v>1.2400446428571431E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>49</v>
       </c>
@@ -1138,7 +1152,7 @@
         <v>68.891369047619051</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D42">
         <f>11/2.5</f>
         <v>4.4000000000000004</v>
@@ -1158,20 +1172,20 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" style="8" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
@@ -1179,7 +1193,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
@@ -1187,7 +1201,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>12</v>
       </c>
@@ -1195,13 +1209,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>40</v>
       </c>
@@ -1209,7 +1223,7 @@
         <v>84.846599999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
@@ -1217,7 +1231,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>41</v>
       </c>
@@ -1225,13 +1239,13 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>17</v>
       </c>
@@ -1239,7 +1253,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>19</v>
       </c>
@@ -1248,7 +1262,7 @@
         <v>4.3611111111111114E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>18</v>
       </c>
@@ -1257,7 +1271,7 @@
         <v>1.7438915287774956E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>20</v>
       </c>
@@ -1265,7 +1279,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>65</v>
       </c>
@@ -1275,7 +1289,7 @@
       </c>
       <c r="E17" s="10"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>9</v>
       </c>
@@ -1290,7 +1304,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>10</v>
       </c>
@@ -1304,7 +1318,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>64</v>
       </c>
@@ -1319,7 +1333,7 @@
         <v>91.55</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>8</v>
       </c>
@@ -1333,7 +1347,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>41</v>
       </c>
@@ -1341,13 +1355,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>67</v>
       </c>
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>35</v>
       </c>
@@ -1355,7 +1369,7 @@
         <v>74.442700000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>36</v>
       </c>
@@ -1363,7 +1377,7 @@
         <v>6.5919999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>37</v>
       </c>
@@ -1371,7 +1385,7 @@
         <v>76.932900000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>38</v>
       </c>
@@ -1379,12 +1393,12 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>32</v>
       </c>
@@ -1400,21 +1414,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R41"/>
+  <dimension ref="B1:R48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
     <col min="9" max="9" width="17" style="24" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" style="24" customWidth="1"/>
     <col min="11" max="11" width="16" style="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>107</v>
       </c>
@@ -1452,12 +1467,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="2:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I2" s="26"/>
       <c r="J2" s="26"/>
       <c r="K2" s="27"/>
     </row>
-    <row r="3" spans="2:18" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
         <v>108</v>
       </c>
@@ -1469,7 +1484,7 @@
         <v>-7.6474000000000002</v>
       </c>
     </row>
-    <row r="4" spans="2:18" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
         <v>109</v>
       </c>
@@ -1481,7 +1496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>53</v>
       </c>
@@ -1508,7 +1523,7 @@
       </c>
       <c r="R5" s="18"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>55</v>
       </c>
@@ -1537,7 +1552,7 @@
       <c r="O6" s="19"/>
       <c r="Q6" s="20"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>54</v>
       </c>
@@ -1566,7 +1581,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>79</v>
       </c>
@@ -1576,7 +1591,7 @@
       <c r="O8" s="20"/>
       <c r="Q8" s="20"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>80</v>
       </c>
@@ -1596,10 +1611,10 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="R10" s="18"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>82</v>
       </c>
@@ -1628,12 +1643,8 @@
       <c r="K11" s="27">
         <v>49.846600000000002</v>
       </c>
-      <c r="O11">
-        <f>K11-K39</f>
-        <v>-48.703399999999995</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>84</v>
       </c>
@@ -1659,7 +1670,7 @@
         <v>49.846600000000002</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>85</v>
       </c>
@@ -1688,49 +1699,29 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15">
+        <v>2.5</v>
+      </c>
+      <c r="I15" s="24">
+        <v>61.994</v>
+      </c>
+      <c r="K15" s="31">
+        <v>54.346600000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>86</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15">
-        <v>50</v>
-      </c>
-      <c r="G15" t="s">
-        <v>62</v>
-      </c>
-      <c r="I15" s="24">
-        <v>77.494</v>
-      </c>
-      <c r="K15" s="25">
-        <v>69.846599999999995</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="E16" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>87</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E17" t="s">
         <v>78</v>
@@ -1747,96 +1738,89 @@
       <c r="K17" s="25">
         <v>69.846599999999995</v>
       </c>
-      <c r="L17">
-        <f>I17-K17</f>
-        <v>7.6474000000000046</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F18">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19">
+        <v>50</v>
+      </c>
+      <c r="G19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" s="24">
+        <v>77.494</v>
+      </c>
+      <c r="K19" s="25">
+        <v>69.846599999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>89</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" t="s">
-        <v>78</v>
-      </c>
-      <c r="F20">
-        <v>40</v>
-      </c>
-      <c r="G20" t="s">
-        <v>90</v>
-      </c>
-      <c r="I20" s="24">
-        <v>94.494</v>
-      </c>
-      <c r="K20" s="25">
-        <v>86.846599999999995</v>
-      </c>
-      <c r="N20" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="E21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F21">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>91</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E22" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F22">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G22" t="s">
         <v>90</v>
       </c>
-      <c r="I22" s="26">
-        <v>98.754000000000005</v>
+      <c r="I22" s="24">
+        <v>94.494</v>
       </c>
       <c r="K22" s="25">
-        <v>98</v>
+        <v>86.846599999999995</v>
       </c>
       <c r="N22" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>79</v>
       </c>
       <c r="F23">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -1851,23 +1835,19 @@
         <v>30</v>
       </c>
       <c r="G24" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="I24" s="26">
-        <v>99.304000000000002</v>
-      </c>
-      <c r="K24" s="27">
-        <v>91.55</v>
-      </c>
-      <c r="L24">
-        <f>K24-K11</f>
-        <v>41.703399999999995</v>
+        <v>98.754000000000005</v>
+      </c>
+      <c r="K24" s="25">
+        <v>98</v>
       </c>
       <c r="N24" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
         <v>79</v>
       </c>
@@ -1875,72 +1855,74 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26">
+        <v>30</v>
+      </c>
+      <c r="G26" t="s">
+        <v>62</v>
+      </c>
+      <c r="I26" s="26">
+        <v>99.304000000000002</v>
+      </c>
+      <c r="K26" s="27">
+        <v>91.55</v>
+      </c>
+      <c r="N26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>93</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" t="s">
-        <v>78</v>
-      </c>
-      <c r="F27">
-        <v>40</v>
-      </c>
-      <c r="G27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="E28" t="s">
-        <v>79</v>
-      </c>
-      <c r="F28">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>94</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E29" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F29">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G29" t="s">
         <v>90</v>
       </c>
-      <c r="I29" s="24">
-        <v>95.557000000000002</v>
-      </c>
-      <c r="K29" s="25">
-        <v>87.909599999999998</v>
-      </c>
-      <c r="M29" s="25"/>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
         <v>79</v>
       </c>
       <c r="F30">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -1955,17 +1937,17 @@
         <v>30</v>
       </c>
       <c r="G31" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="I31" s="24">
-        <v>96.156999999999996</v>
+        <v>95.557000000000002</v>
       </c>
       <c r="K31" s="25">
-        <v>88.509600000000006</v>
+        <v>87.909599999999998</v>
       </c>
       <c r="M31" s="25"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
         <v>79</v>
       </c>
@@ -1973,72 +1955,84 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" t="s">
+        <v>81</v>
+      </c>
+      <c r="F33">
+        <v>30</v>
+      </c>
+      <c r="G33" t="s">
+        <v>62</v>
+      </c>
+      <c r="I33" s="24">
+        <v>96.156999999999996</v>
+      </c>
+      <c r="K33" s="25">
+        <v>88.509600000000006</v>
+      </c>
+      <c r="M33" s="25"/>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>96</v>
       </c>
-      <c r="C34">
+      <c r="C36">
         <v>2.5</v>
-      </c>
-      <c r="D34" t="s">
-        <v>83</v>
-      </c>
-      <c r="E34" t="s">
-        <v>81</v>
-      </c>
-      <c r="F34">
-        <v>40</v>
-      </c>
-      <c r="G34" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
       </c>
       <c r="D36" t="s">
         <v>83</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F36">
         <v>40</v>
       </c>
       <c r="G36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" t="s">
+        <v>78</v>
+      </c>
+      <c r="F38">
+        <v>40</v>
+      </c>
+      <c r="G38" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>99</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37" t="s">
-        <v>83</v>
-      </c>
-      <c r="E37" t="s">
-        <v>81</v>
-      </c>
-      <c r="F37">
-        <v>40</v>
-      </c>
-      <c r="G37" t="s">
-        <v>62</v>
-      </c>
-      <c r="M37" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
-        <v>100</v>
       </c>
       <c r="C39">
         <v>2</v>
@@ -2050,44 +2044,18 @@
         <v>81</v>
       </c>
       <c r="F39">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G39" t="s">
         <v>62</v>
       </c>
-      <c r="K39" s="25">
-        <v>98.55</v>
-      </c>
       <c r="M39" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
-        <v>101</v>
-      </c>
-      <c r="C40">
-        <v>2</v>
-      </c>
-      <c r="D40" t="s">
-        <v>77</v>
-      </c>
-      <c r="E40" t="s">
-        <v>81</v>
-      </c>
-      <c r="F40">
-        <v>30</v>
-      </c>
-      <c r="G40" t="s">
-        <v>90</v>
-      </c>
-      <c r="M40" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C41">
         <v>2</v>
@@ -2102,10 +2070,104 @@
         <v>30</v>
       </c>
       <c r="G41" t="s">
-        <v>90</v>
+        <v>62</v>
+      </c>
+      <c r="K41" s="25">
+        <v>98.55</v>
       </c>
       <c r="M41" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" t="s">
+        <v>81</v>
+      </c>
+      <c r="F42">
+        <v>30</v>
+      </c>
+      <c r="G42" t="s">
+        <v>90</v>
+      </c>
+      <c r="M42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>83</v>
+      </c>
+      <c r="E43" t="s">
+        <v>81</v>
+      </c>
+      <c r="F43">
+        <v>30</v>
+      </c>
+      <c r="G43" t="s">
+        <v>90</v>
+      </c>
+      <c r="M43" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45">
+        <v>90</v>
+      </c>
+      <c r="I45" s="24">
+        <v>66.396000000000001</v>
+      </c>
+      <c r="K45" s="25">
+        <v>58.748600000000003</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46">
+        <v>90</v>
+      </c>
+      <c r="I46" s="24">
+        <f>74.668+0.3</f>
+        <v>74.968000000000004</v>
+      </c>
+      <c r="K46" s="25">
+        <f>67.0206+0.3</f>
+        <v>67.320599999999999</v>
+      </c>
+      <c r="L46">
+        <f>K45-K46</f>
+        <v>-8.5719999999999956</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48">
+        <v>90</v>
+      </c>
+      <c r="K48" s="24">
+        <v>45.939799999999998</v>
       </c>
     </row>
   </sheetData>
@@ -2122,12 +2184,12 @@
       <selection sqref="A1:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>51</v>
       </c>
@@ -2138,7 +2200,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
         <v>11</v>
       </c>
@@ -2146,7 +2208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>53</v>
       </c>
@@ -2154,7 +2216,7 @@
         <v>48.0901</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>54</v>
       </c>
@@ -2166,7 +2228,7 @@
         <v>41.442700000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>56</v>
       </c>
@@ -2177,7 +2239,7 @@
         <v>49.846600000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
         <v>57</v>
       </c>
@@ -2192,7 +2254,7 @@
         <v>28.403899999999993</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -2210,7 +2272,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -2228,7 +2290,7 @@
         <v>4.1534000000000049</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>61</v>
       </c>

</xml_diff>